<commit_message>
comparison graphs for pp 10-fold
</commit_message>
<xml_diff>
--- a/results/comparisons/pre-processing-impact/pp-10Fold.xlsx
+++ b/results/comparisons/pre-processing-impact/pp-10Fold.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="42820" windowHeight="23700" tabRatio="990"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Avg" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t>Ranking 101 datasets</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Rank with best ordered like with p11</t>
+  </si>
+  <si>
+    <t>Accuracy with best ordered like with p11</t>
   </si>
 </sst>
 </file>
@@ -388,35 +394,1849 @@
     </xf>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Rank with p11</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Avg!$A$9:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>Svm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RotationForest J48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logistic Model Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RotationForest RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bagging PART</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bagging J48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MultiboostAB J48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MultiboostAB NBTree</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MultiboostAB, PART</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>AdaboostM1, J48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bagging NBTree</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Multillayer Perceptron</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MultiboostAB JRip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Bagging RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MultiboostAB, RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bagging JRip</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomComittee RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Classification ViaRegression, M5P</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Decorate</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Simple Logistic</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Bagging RepTree</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Alternating Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>MultiboostAB, RepTree</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>PART</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Smo</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>NBTree</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>OrdinalClassClassifier J48</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>JRip</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Random Subspaces of RepTree</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>DTNB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>MultiboostAB, Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>RBF Network</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>IBk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Ridor</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Rep Tree</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Bagging Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>MultiboostAB, Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>IB1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Dagging SMO</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Random Tree</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Bagging Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Bagging LWL</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>LogitBoost Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>LWL</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>VFI</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>AdaboostM1, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>MultiboostAB DecisionStump</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Bagging Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Bagging Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Conjunctive Rule</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>NNge</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Classification via Clustering: FarthestFirst</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Classification via Clustering: KMeans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Avg!$B$9:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>33.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Rank with best pi</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Avg!$A$9:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>Svm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RotationForest J48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logistic Model Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RotationForest RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bagging PART</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bagging J48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MultiboostAB J48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MultiboostAB NBTree</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MultiboostAB, PART</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>AdaboostM1, J48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bagging NBTree</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Multillayer Perceptron</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MultiboostAB JRip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Bagging RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MultiboostAB, RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bagging JRip</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomComittee RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Classification ViaRegression, M5P</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Decorate</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Simple Logistic</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Bagging RepTree</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Alternating Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>MultiboostAB, RepTree</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>PART</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Smo</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>NBTree</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>OrdinalClassClassifier J48</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>JRip</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Random Subspaces of RepTree</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>DTNB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>MultiboostAB, Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>RBF Network</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>IBk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Ridor</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Rep Tree</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Bagging Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>MultiboostAB, Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>IB1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Dagging SMO</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Random Tree</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Bagging Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Bagging LWL</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>LogitBoost Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>LWL</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>VFI</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>AdaboostM1, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>MultiboostAB DecisionStump</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Bagging Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Bagging Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Conjunctive Rule</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>NNge</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Classification via Clustering: FarthestFirst</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Classification via Clustering: KMeans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Avg!$N$9:$N$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>31.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2121073128"/>
+        <c:axId val="2121075432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2121073128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121075432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121075432"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:min val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121073128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Avg accuracy with p11</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Avg!$A$9:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>Svm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RotationForest J48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logistic Model Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RotationForest RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bagging PART</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bagging J48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MultiboostAB J48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MultiboostAB NBTree</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MultiboostAB, PART</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>AdaboostM1, J48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bagging NBTree</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Multillayer Perceptron</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MultiboostAB JRip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Bagging RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MultiboostAB, RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bagging JRip</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomComittee RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Classification ViaRegression, M5P</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Decorate</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Simple Logistic</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Bagging RepTree</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Alternating Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>MultiboostAB, RepTree</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>PART</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Smo</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>NBTree</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>OrdinalClassClassifier J48</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>JRip</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Random Subspaces of RepTree</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>DTNB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>MultiboostAB, Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>RBF Network</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>IBk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Ridor</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Rep Tree</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Bagging Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>MultiboostAB, Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>IB1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Dagging SMO</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Random Tree</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Bagging Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Bagging LWL</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>LogitBoost Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>LWL</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>VFI</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>AdaboostM1, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>MultiboostAB DecisionStump</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Bagging Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Bagging Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Conjunctive Rule</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>NNge</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Classification via Clustering: FarthestFirst</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Classification via Clustering: KMeans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Avg!$C$9:$C$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>0.764821846304509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76448881370627</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.759890063490698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.759255535420912</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.757725393765826</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.753996835814947</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.750954296788182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75071741822896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.750685513034466</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.749660788966091</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.748897685543846</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.748684644448501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.748008862878428</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.746342639811875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.746175767564358</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.745695995836934</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.743839245371165</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.743819150683958</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.743520090291786</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.743431213905039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.742827356858684</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.73913246567437</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.737718651504176</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.737517973481584</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.734658459853298</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.731966222728814</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.729948403120064</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.727387690136033</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.725721305042599</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.724015824274423</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.722978119405648</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.722152911870206</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.721086965253612</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.718885243220091</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.717571438243912</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.716208484681389</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.714991537954213</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.714646326333884</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.712002021739229</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.710234622802721</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.710192524615728</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.706047752564169</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.705123245160407</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.703143731617964</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.699997654948603</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.691984342005588</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.661735703075628</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.654589105464886</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.640445235752752</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.634032030447139</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.622292523721582</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.616321851447554</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.615403687903945</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.598959701498148</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.589813240844951</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.580599257146857</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.573567983305147</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.533560795692168</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.517611177330317</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.51339631645015</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.504376199542545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Avg accuracy with p11</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Avg!$A$9:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>Svm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RotationForest J48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logistic Model Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RotationForest RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bagging PART</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bagging J48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MultiboostAB J48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MultiboostAB NBTree</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MultiboostAB, PART</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>AdaboostM1, J48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bagging NBTree</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Multillayer Perceptron</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MultiboostAB JRip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Bagging RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MultiboostAB, RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bagging JRip</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomComittee RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Classification ViaRegression, M5P</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Decorate</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Simple Logistic</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Bagging RepTree</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Alternating Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>MultiboostAB, RepTree</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>PART</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Smo</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>NBTree</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>OrdinalClassClassifier J48</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>JRip</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Random Subspaces of RepTree</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>DTNB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>MultiboostAB, Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>RBF Network</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>IBk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Ridor</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Rep Tree</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Bagging Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>MultiboostAB, Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>IB1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Dagging SMO</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Random Tree</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Bagging Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Bagging LWL</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>LogitBoost Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>LWL</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>VFI</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>AdaboostM1, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>MultiboostAB DecisionStump</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Bagging Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Bagging Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Hyper Pipes</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Conjunctive Rule</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>NNge</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Classification via Clustering: FarthestFirst</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Classification via Clustering: KMeans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Avg!$O$9:$O$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>0.803861580781583</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.801159056812684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.795701517463844</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79802149096821</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.798909854589839</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.787882792115231</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.781110537075631</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.790095867161159</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.791840827420044</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.788693294177632</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.787699799562187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.79064840750636</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.791734619679964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78564239818109</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.784990651502447</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.784959127468532</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.780871091171926</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.787097552440233</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.771767545416136</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.773799585287673</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.776262098677396</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.766200541641526</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.779891937841556</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.773697297775359</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.769354472322416</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.771260775559199</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.770490144553752</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.75696654197554</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.777994839271978</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.761280059287879</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.769904014224627</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.764357344358126</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.774780660242716</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.759789274755294</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.759423712202328</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.77503578573429</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.758970190126839</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.749681826302667</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.749584300038882</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.776565199087507</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.760954229449681</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.747158522034617</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.774251116675412</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.756338375944413</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.77279505006462</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.736293723228252</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.716124277836516</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.686466405779222</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.703535934127426</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.744002632073688</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.659761332131493</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.650239278975321</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.670124187109935</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.631956200835068</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.633442317232121</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.612535303746812</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.602631096512144</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.541064698658286</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.717707785280581</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.600707996742875</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.620778628936991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2116332984"/>
+        <c:axId val="2120042840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2116332984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120042840"/>
+        <c:crossesAt val="0.49"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2120042840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.82"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2116332984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.05"/>
+        <c:minorUnit val="0.001"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>183662</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>79130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -741,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -757,9 +2577,11 @@
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13">
+    <row r="1" spans="1:15" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13">
+    <row r="3" spans="1:15" ht="13">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -775,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13">
+    <row r="5" spans="1:15" ht="13">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -790,7 +2612,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -801,7 +2623,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -833,8 +2655,14 @@
       <c r="L7" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="N7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -845,7 +2673,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -879,8 +2707,16 @@
         <f t="shared" ref="L9:L52" si="0">INDEX(A$9:I$69,MATCH(F9,A$9:A$69,0),3)</f>
         <v>0.764821846304509</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9">
+        <f>INDEX(A$9:I$73,MATCH(A9,F$9:F$73,0),7)</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f>INDEX(A$9:J$73,MATCH(A9,F$9:F$73,0),8)</f>
+        <v>0.80386158078158299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -914,8 +2750,16 @@
         <f t="shared" si="0"/>
         <v>0.76448881370626998</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="N10">
+        <f t="shared" ref="N10:N69" si="2">INDEX(A$9:I$73,MATCH(A10,F$9:F$73,0),7)</f>
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ref="O10:O69" si="3">INDEX(A$9:J$73,MATCH(A10,F$9:F$73,0),8)</f>
+        <v>0.80115905681268396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -949,8 +2793,16 @@
         <f t="shared" si="0"/>
         <v>0.75772539376582604</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>0.79570151746384399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -984,8 +2836,16 @@
         <f t="shared" si="0"/>
         <v>0.75925553542091195</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>0.79802149096820996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1019,8 +2879,16 @@
         <f t="shared" si="0"/>
         <v>0.75989006349069799</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>0.79890985458983899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1054,8 +2922,16 @@
         <f t="shared" si="0"/>
         <v>0.75068551303446596</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>0.78788279211523105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1089,8 +2965,16 @@
         <f t="shared" si="0"/>
         <v>0.74800886287842805</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>0.78111053707563105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1124,8 +3008,16 @@
         <f t="shared" si="0"/>
         <v>0.74868464444850102</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>0.79009586716115898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1159,8 +3051,16 @@
         <f t="shared" si="0"/>
         <v>0.75071741822895999</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>0.79184082742004402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1194,8 +3094,16 @@
         <f t="shared" si="0"/>
         <v>0.74966078896609101</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>0.78869329417763201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1229,8 +3137,16 @@
         <f t="shared" si="0"/>
         <v>0.75399683581494703</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>0.78769979956218705</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1264,8 +3180,16 @@
         <f t="shared" si="0"/>
         <v>0.74889768554384595</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>0.79064840750636001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1299,8 +3223,16 @@
         <f t="shared" si="0"/>
         <v>0.74381915068395799</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="3"/>
+        <v>0.79173461967996395</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1334,8 +3266,16 @@
         <f t="shared" si="0"/>
         <v>0.74634263981187499</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="3"/>
+        <v>0.78564239818109005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1369,8 +3309,16 @@
         <f t="shared" si="0"/>
         <v>0.74617576756435799</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="3"/>
+        <v>0.78499065150244696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1404,8 +3352,16 @@
         <f t="shared" si="0"/>
         <v>0.74569599583693402</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="3"/>
+        <v>0.78495912746853203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1439,8 +3395,16 @@
         <f t="shared" si="0"/>
         <v>0.75095429678818204</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>0.78087109117192599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -1474,8 +3438,16 @@
         <f t="shared" si="0"/>
         <v>0.74383924537116497</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="3"/>
+        <v>0.78709755244023305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1509,8 +3481,16 @@
         <f t="shared" si="0"/>
         <v>0.73771865150417604</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>0.77176754541613601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1544,8 +3524,16 @@
         <f t="shared" si="0"/>
         <v>0.72572130504259902</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="3"/>
+        <v>0.77379958528767301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1579,8 +3567,16 @@
         <f t="shared" si="0"/>
         <v>0.71023462280272098</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="3"/>
+        <v>0.77626209867739604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1614,8 +3610,16 @@
         <f t="shared" si="0"/>
         <v>0.74282735685868395</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>0.76620054164152596</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1649,8 +3653,16 @@
         <f t="shared" si="0"/>
         <v>0.71620848468138898</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="3"/>
+        <v>0.77989193784155597</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1684,8 +3696,16 @@
         <f t="shared" si="0"/>
         <v>0.72108696525361204</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="3"/>
+        <v>0.77369729777535901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1719,8 +3739,16 @@
         <f t="shared" si="0"/>
         <v>0.70512324516040703</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="3"/>
+        <v>0.76935447232241605</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1754,8 +3782,16 @@
         <f t="shared" si="0"/>
         <v>0.74343121390503897</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="3"/>
+        <v>0.77126077555919903</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1789,8 +3825,16 @@
         <f t="shared" si="0"/>
         <v>0.73751797348158399</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="3"/>
+        <v>0.77049014455375198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1824,8 +3868,16 @@
         <f t="shared" si="0"/>
         <v>0.699997654948603</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>0.75696654197554003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
@@ -1859,8 +3911,16 @@
         <f t="shared" si="0"/>
         <v>0.74352009029178601</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>0.77799483927197799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1894,8 +3954,16 @@
         <f t="shared" si="0"/>
         <v>0.73196622272881395</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>0.76128005928787901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1929,8 +3997,16 @@
         <f t="shared" si="0"/>
         <v>0.72994840312006404</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>0.76990401422462695</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1964,8 +4040,16 @@
         <f t="shared" si="0"/>
         <v>0.72297811940564805</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>0.76435734435812597</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
@@ -1999,8 +4083,16 @@
         <f t="shared" si="0"/>
         <v>0.73465845985329803</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="3"/>
+        <v>0.77478066024271597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
         <v>45</v>
       </c>
@@ -2034,8 +4126,16 @@
         <f t="shared" si="0"/>
         <v>0.73913246567436997</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="3"/>
+        <v>0.75978927475529401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
@@ -2069,8 +4169,16 @@
         <f t="shared" si="0"/>
         <v>0.72215291187020603</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="3"/>
+        <v>0.75942371220232796</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="2" t="s">
         <v>33</v>
       </c>
@@ -2104,8 +4212,16 @@
         <f t="shared" si="0"/>
         <v>0.72401582427442301</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="3"/>
+        <v>0.77503578573428999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -2139,8 +4255,16 @@
         <f t="shared" si="0"/>
         <v>0.71019252461572802</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="3"/>
+        <v>0.75897019012683897</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="2" t="s">
         <v>49</v>
       </c>
@@ -2174,8 +4298,16 @@
         <f t="shared" si="0"/>
         <v>0.71888524322009095</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="3"/>
+        <v>0.749681826302667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="2" t="s">
         <v>50</v>
       </c>
@@ -2209,8 +4341,16 @@
         <f t="shared" si="0"/>
         <v>0.71757143824391201</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="3"/>
+        <v>0.74958430003888199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="2" t="s">
         <v>31</v>
       </c>
@@ -2244,8 +4384,16 @@
         <f t="shared" si="0"/>
         <v>0.714991537954213</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="3"/>
+        <v>0.77656519908750699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2279,8 +4427,16 @@
         <f t="shared" si="0"/>
         <v>0.72738769013603299</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="3"/>
+        <v>0.76095422944968105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -2314,8 +4470,16 @@
         <f t="shared" si="0"/>
         <v>0.70314373161796395</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="3"/>
+        <v>0.74715852203461697</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
@@ -2349,8 +4513,16 @@
         <f t="shared" si="0"/>
         <v>0.71464632633388403</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="3"/>
+        <v>0.77425111667541202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -2384,8 +4556,16 @@
         <f t="shared" si="0"/>
         <v>0.712002021739229</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="3"/>
+        <v>0.756338375944413</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="2" t="s">
         <v>41</v>
       </c>
@@ -2412,15 +4592,23 @@
         <v>0.20518818535969199</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" ref="K53:K69" si="2">IF(L53&gt;0,H53-L53,"?")</f>
+        <f t="shared" ref="K53:K69" si="4">IF(L53&gt;0,H53-L53,"?")</f>
         <v>4.1110769470448005E-2</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" ref="L53:L69" si="3">INDEX(A$9:I$69,MATCH(F53,A$9:A$69,0),3)</f>
+        <f t="shared" ref="L53:L69" si="5">INDEX(A$9:I$69,MATCH(F53,A$9:A$69,0),3)</f>
         <v>0.70604775256416896</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="3"/>
+        <v>0.77279505006462001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2447,15 +4635,23 @@
         <v>0.18419336304504699</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10997060162654904</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.63403203044713896</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="3"/>
+        <v>0.73629372322825204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2482,15 +4678,23 @@
         <v>0.18053292168335999</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4309381222664035E-2</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.691984342005588</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="3"/>
+        <v>0.716124277836516</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -2517,15 +4721,23 @@
         <v>0.190946452072777</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20009660795026396</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.51761117733031703</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="3"/>
+        <v>0.68646640577922202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -2552,15 +4764,23 @@
         <v>0.19598146455742901</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.4388574760887987E-2</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.66173570307562801</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="3"/>
+        <v>0.70353593412742599</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="2" t="s">
         <v>54</v>
       </c>
@@ -2587,15 +4807,23 @@
         <v>0.20248570099477201</v>
       </c>
       <c r="K58" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3090698374673959E-2</v>
       </c>
       <c r="L58" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.64044523575275203</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="3"/>
+        <v>0.744002632073688</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="2" t="s">
         <v>59</v>
       </c>
@@ -2622,15 +4850,23 @@
         <v>0.18321196884152299</v>
       </c>
       <c r="K59" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.1877300314335999E-2</v>
       </c>
       <c r="L59" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.65458910546488602</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="3"/>
+        <v>0.65976133213149302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -2657,15 +4893,23 @@
         <v>0.20492893659662501</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.4720499205990092E-2</v>
       </c>
       <c r="L60" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.61540368790394495</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="3"/>
+        <v>0.65023927897532097</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="2" t="s">
         <v>61</v>
       </c>
@@ -2692,15 +4936,23 @@
         <v>0.251400451794214</v>
       </c>
       <c r="K61" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.746880840991107E-2</v>
       </c>
       <c r="L61" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.62229252372158195</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="N61">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="3"/>
+        <v>0.67012418710993504</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
         <v>62</v>
       </c>
@@ -2727,15 +4979,23 @@
         <v>0.24419012306752499</v>
       </c>
       <c r="K62" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3917427527766941E-2</v>
       </c>
       <c r="L62" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.61632185144755403</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="N62">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="3"/>
+        <v>0.63195620083506798</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -2762,15 +5022,23 @@
         <v>0.216672953162696</v>
       </c>
       <c r="K63" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.3629076387169952E-2</v>
       </c>
       <c r="L63" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.58981324084495101</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="N63">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="3"/>
+        <v>0.63344231723212097</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -2797,15 +5065,23 @@
         <v>0.22542669427662801</v>
       </c>
       <c r="K64" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2996499336919949E-2</v>
       </c>
       <c r="L64" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.59895970149814803</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="N64">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="3"/>
+        <v>0.61253530374681198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -2832,15 +5108,23 @@
         <v>0.191302187750649</v>
       </c>
       <c r="K65" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.11640242939444601</v>
       </c>
       <c r="L65" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.50437619954254498</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="N65">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="3"/>
+        <v>0.60263109651214397</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -2867,15 +5151,23 @@
         <v>0.24184395566431999</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.193604659995497E-2</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.58059925714685701</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="N66">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="3"/>
+        <v>0.54106469865828599</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="2" t="s">
         <v>57</v>
       </c>
@@ -2902,15 +5194,23 @@
         <v>0.24652885390363999</v>
       </c>
       <c r="K67" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9063113206996949E-2</v>
       </c>
       <c r="L67" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57356798330514702</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="N67">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="3"/>
+        <v>0.71770778528058099</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -2937,15 +5237,23 @@
         <v>0.20880837218004999</v>
       </c>
       <c r="K68" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.7311680292724958E-2</v>
       </c>
       <c r="L68" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.51339631645015005</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="N68">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="3"/>
+        <v>0.60070799674287501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
@@ -2972,15 +5280,23 @@
         <v>0.29320675458551199</v>
       </c>
       <c r="K69" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.5039029661180257E-3</v>
       </c>
       <c r="L69" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.53356079569216797</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="N69">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="3"/>
+        <v>0.62077862893699098</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="B71" s="4" t="s">
         <v>71</v>
       </c>
@@ -3003,7 +5319,7 @@
         <v>4.6908029828947984E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:15">
       <c r="J72" s="4" t="s">
         <v>72</v>
       </c>
@@ -3012,7 +5328,7 @@
         <v>7.5039029661180257E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:15">
       <c r="J73" s="4" t="s">
         <v>73</v>
       </c>
@@ -3023,7 +5339,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>